<commit_message>
Edit No cargo cmt
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -5924,7 +5924,7 @@
       </c>
       <c r="AAF24" s="92" t="inlineStr">
         <is>
-          <t>No cargo: FPREMOU001SWENEOBORAMTEKBUENO</t>
+          <t>No cargo: FPREMOU001BUENOSWENEOBORAMTEK</t>
         </is>
       </c>
       <c r="AAG24" s="92" t="n"/>
@@ -6548,7 +6548,7 @@
       </c>
       <c r="AAF28" s="92" t="inlineStr">
         <is>
-          <t xml:space="preserve">No cargo: GIAVICO , CHANGHONG , PHTHAP02 , LILOIN01 , LAMNGHIEP , CNACHAU , KIMBUU , </t>
+          <t xml:space="preserve">No cargo: GIAVICO , CHANGHONG , PHTHAP02 , LILOIN01 , KIMBUU , POWERBEST , LAMNGHIEP , </t>
         </is>
       </c>
       <c r="AAG28" s="92" t="n"/>
@@ -7638,7 +7638,7 @@
       <c r="ZW32" s="66" t="n"/>
       <c r="AAF32" s="92" t="inlineStr">
         <is>
-          <t xml:space="preserve">No cargo: CN0171 , COTYTN524 , TLAPTHANH , ITIHCM , MINHDANG , TSCAMAU , COTYCO92 , </t>
+          <t xml:space="preserve">No cargo: CN0171 , ITIHCM , TLAPTHANH , COTYTN524 , MINHDANG , COTYCO92 , TSCAMAU , </t>
         </is>
       </c>
       <c r="AAG32" s="92" t="n"/>

</xml_diff>